<commit_message>
Add newly generated charts and maps
</commit_message>
<xml_diff>
--- a/daily_aqi_data/SL_Daily_AQI_2025-02-08.xlsx
+++ b/daily_aqi_data/SL_Daily_AQI_2025-02-08.xlsx
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
@@ -10500,7 +10500,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>

</xml_diff>